<commit_message>
test concurrent req download
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -44,22 +44,22 @@
     <t>Price/Sales</t>
   </si>
   <si>
-    <t>CRWD</t>
-  </si>
-  <si>
-    <t>487.83M -&gt; 535.15M -&gt; 580.88M -&gt; 637.37M -&gt; 692.58M</t>
-  </si>
-  <si>
-    <t>-0.14 -&gt; -0.21 -&gt; -0.24 -&gt; -0.2 -&gt; 0.0</t>
-  </si>
-  <si>
-    <t>159.74M -&gt; 138.25M -&gt; 176.41M -&gt; 212.85M -&gt; 230.93M</t>
-  </si>
-  <si>
-    <t>1.61 &lt;- 1.22 &lt;- 2.19 &lt;- 3.79 &lt;- 4.63</t>
-  </si>
-  <si>
-    <t>12.49 &lt;- 12.06 &lt;- 20.25 &lt;- 25.68 &lt;- 31.10</t>
+    <t>NET</t>
+  </si>
+  <si>
+    <t>212.17M -&gt; 234.52M -&gt; 253.86M -&gt; 274.7M -&gt; 290.18M</t>
+  </si>
+  <si>
+    <t>-0.13 -&gt; -0.2 -&gt; -0.13 -&gt; -0.14 -&gt; -0.12</t>
+  </si>
+  <si>
+    <t>(54.95M) -&gt; 6.65M -&gt; 6.13M -&gt; 34.08M -&gt; 20.81M</t>
+  </si>
+  <si>
+    <t>5.75 &lt;- N/A &lt;- N/A &lt;- N/A</t>
+  </si>
+  <si>
+    <t>20.63 &lt;- 16.39 &lt;- 21.85 &lt;- 18.96</t>
   </si>
   <si>
     <t>EPS Estimate</t>
@@ -80,16 +80,16 @@
     <t>Price Delta</t>
   </si>
   <si>
-    <t>0.51</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>55900, 402</t>
-  </si>
-  <si>
-    <t>35, 35</t>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>158, 157</t>
+  </si>
+  <si>
+    <t>30, 31</t>
   </si>
 </sst>
 </file>
@@ -460,14 +460,14 @@
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1">
@@ -507,19 +507,19 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="2">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -584,7 +584,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -593,7 +593,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="2">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>